<commit_message>
Hosts a database, pulls info from database, and can take new entries
</commit_message>
<xml_diff>
--- a/src/main/webapp/assets/MoviesJavaWebProgrammingSheet.xlsx
+++ b/src/main/webapp/assets/MoviesJavaWebProgrammingSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caseybement/Desktop/CVTC/Java Web Programming/Movies_CBement/src/main/webapp/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3CC5B4-2A1D-1148-80FE-93231FAC78A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE706A73-EF97-9B4B-B3F0-C123C515B735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="1000" windowWidth="26340" windowHeight="15180" xr2:uid="{0C1AEBEF-6521-2946-B4E4-9D3408CE8296}"/>
   </bookViews>
@@ -115,12 +115,10 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,17 +138,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,7 +470,7 @@
     <col min="4" max="4" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,9 +556,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" xr:uid="{3C437845-D76F-4C40-B476-5D7A0CB08CC4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>